<commit_message>
Modificacion de documentos de Pruebas Funcionales 25/11/23
</commit_message>
<xml_diff>
--- a/Tester/SRSPG_Pruebas_de_Aceptación.xlsx
+++ b/Tester/SRSPG_Pruebas_de_Aceptación.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanC\OneDrive\Escritorio\proyecto 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanC\OneDrive\Escritorio\2023.2\proyecto 1\Proyecto-I\Tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB83C48-0F8B-4CCB-A5CB-B8172B503B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2D89EE-4B35-4B72-A2CF-E04788C398AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="1" activeTab="3" xr2:uid="{9370D1F1-6C14-4FB8-9272-9D8C43E5B414}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="37">
   <si>
     <t>Número del Caso de Prueba</t>
   </si>
@@ -203,6 +203,15 @@
   </si>
   <si>
     <t>CP011</t>
+  </si>
+  <si>
+    <t>El usuario Profesor debe poder crear propuestas de trabajo de grado, de modo que estas se publiquen.</t>
+  </si>
+  <si>
+    <t>El usuario director del trabajo de grado debe poder registrar los datos necesarios para registrar (enviar) el trabajo de grado.</t>
+  </si>
+  <si>
+    <t>Un profesor o usuario con los permisos de director de trabajo debe poder registrar el anteproyecto en el sistema</t>
   </si>
 </sst>
 </file>
@@ -422,22 +431,23 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -446,7 +456,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -779,127 +788,127 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="2:9" ht="16.5">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
     </row>
     <row r="4" spans="2:9" ht="16.5">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" spans="2:9" ht="16.5">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
     </row>
     <row r="8" spans="2:9" ht="18.75" thickBot="1">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
     </row>
     <row r="9" spans="2:9" s="5" customFormat="1" ht="54" customHeight="1" thickTop="1">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="11"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9" t="s">
+      <c r="G9" s="11"/>
+      <c r="H9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="9"/>
+      <c r="I9" s="11"/>
     </row>
     <row r="10" spans="2:9" ht="89.25">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="12"/>
+      <c r="C10" s="14"/>
       <c r="D10" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="13"/>
+      <c r="G10" s="9"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="2:9" ht="89.25">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="12"/>
+      <c r="C11" s="14"/>
       <c r="D11" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="13"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="2:9" ht="16.5">
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="3"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="13"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="2:9" ht="191.25">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="13"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
     </row>
@@ -930,26 +939,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="F10:G10"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H11:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -960,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2633ACA9-8603-4095-B2DA-7E9864DEC261}">
   <dimension ref="B2:I18"/>
   <sheetViews>
-    <sheetView zoomScale="43" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView topLeftCell="A9" zoomScale="65" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -975,122 +984,124 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="2:9" ht="16.5">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
     </row>
     <row r="4" spans="2:9" ht="16.5">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" spans="2:9" ht="16.5">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
     </row>
     <row r="8" spans="2:9" ht="18.75" thickBot="1">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
     </row>
     <row r="9" spans="2:9" s="5" customFormat="1" ht="54" customHeight="1" thickTop="1">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="11"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9" t="s">
+      <c r="G9" s="11"/>
+      <c r="H9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="9"/>
+      <c r="I9" s="11"/>
     </row>
     <row r="10" spans="2:9" ht="89.25">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="12"/>
+      <c r="C10" s="14"/>
       <c r="D10" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="13"/>
+      <c r="G10" s="9"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="2:9" ht="16.5">
-      <c r="B11" s="12" t="s">
+    <row r="11" spans="2:9" ht="42.75">
+      <c r="B11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="3"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="13"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="2:9" ht="16.5">
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="3"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="13"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="2:9" ht="16.5">
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="3"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="13"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="2:9">
-      <c r="E14" s="16"/>
+      <c r="E14" s="8"/>
     </row>
     <row r="15" spans="2:9" ht="15.75">
       <c r="B15" s="2" t="s">
@@ -1119,17 +1130,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="H11:I11"/>
@@ -1139,6 +1139,17 @@
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:C9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1163,103 +1174,103 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="2:9" ht="16.5">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
     </row>
     <row r="4" spans="2:9" ht="16.5">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" spans="2:9" ht="16.5">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
     </row>
     <row r="8" spans="2:9" ht="18.75" thickBot="1">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
     </row>
     <row r="9" spans="2:9" s="5" customFormat="1" ht="54" customHeight="1" thickTop="1">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="11"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9" t="s">
+      <c r="G9" s="11"/>
+      <c r="H9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="9"/>
+      <c r="I9" s="11"/>
     </row>
     <row r="10" spans="2:9" ht="89.25">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="12"/>
+      <c r="C10" s="14"/>
       <c r="D10" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="13"/>
+      <c r="G10" s="9"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="2:9" ht="16.5">
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="13"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
     </row>
     <row r="13" spans="2:9" ht="16.5">
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="3"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="13"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
     </row>
@@ -1290,6 +1301,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B8:D8"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="H13:I13"/>
@@ -1301,11 +1317,6 @@
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1316,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F14AD65-0BF0-4F9E-8729-C3B71F7205F6}">
   <dimension ref="B2:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="58" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:C13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="79" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1331,119 +1342,123 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="2:9" ht="16.5">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
     </row>
     <row r="4" spans="2:9" ht="16.5">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" spans="2:9" ht="16.5">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
     </row>
     <row r="8" spans="2:9" ht="18.75" thickBot="1">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
     </row>
     <row r="9" spans="2:9" s="5" customFormat="1" ht="54" customHeight="1" thickTop="1">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="11"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9" t="s">
+      <c r="G9" s="11"/>
+      <c r="H9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="9"/>
+      <c r="I9" s="11"/>
     </row>
     <row r="10" spans="2:9" ht="102">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="12"/>
+      <c r="C10" s="14"/>
       <c r="D10" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="13"/>
+      <c r="G10" s="9"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="2:9" ht="16.5">
-      <c r="B11" s="12" t="s">
+    <row r="11" spans="2:9" ht="61.5" customHeight="1">
+      <c r="B11" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="3"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="13"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="2:9" ht="16.5">
-      <c r="B12" s="12" t="s">
+    <row r="12" spans="2:9" ht="68.25" customHeight="1">
+      <c r="B12" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="3"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="E12" s="6"/>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="13"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="2:9" ht="16.5">
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="3"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="13"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
     </row>
@@ -1474,17 +1489,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="H11:I11"/>
@@ -1494,6 +1498,17 @@
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:C9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modificacion de documentos de Pruebas Funcionales y de aceptacion 27/11/23
</commit_message>
<xml_diff>
--- a/Tester/SRSPG_Pruebas_de_Aceptación.xlsx
+++ b/Tester/SRSPG_Pruebas_de_Aceptación.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanC\OneDrive\Escritorio\2023.2\proyecto 1\Proyecto-I\Tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2D89EE-4B35-4B72-A2CF-E04788C398AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8247088E-D73A-451A-BA14-D6263ED87F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="1" activeTab="3" xr2:uid="{9370D1F1-6C14-4FB8-9272-9D8C43E5B414}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{9370D1F1-6C14-4FB8-9272-9D8C43E5B414}"/>
   </bookViews>
   <sheets>
     <sheet name="PruebasAceptacion_Jefatura" sheetId="1" r:id="rId1"/>
     <sheet name="Usuario=Profesor" sheetId="2" r:id="rId2"/>
-    <sheet name="Usuario=Estudiante" sheetId="3" r:id="rId3"/>
-    <sheet name="Usuario=Director de TrabGrado" sheetId="4" r:id="rId4"/>
+    <sheet name="Usuario=Concejo de facultad" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
   <si>
     <t>Número del Caso de Prueba</t>
   </si>
@@ -150,20 +149,6 @@
     <t>CP012</t>
   </si>
   <si>
-    <t>CP05</t>
-  </si>
-  <si>
-    <t>El usuario Estudiante debe poder iniciar sesión en la aplicación para poder acceder a sus funcionalidades.</t>
-  </si>
-  <si>
-    <t>1. El sistema debe proporcionar un campo de entrada de usuario y contraseña en la página de inicio de sesión.
-2. Los usuarios deben poder ingresar su correo y contraseña en los campos correspondientes.
-3. El sistema debe verificar las credenciales proporcionadas por el usuario y autenticar con éxito a los usuarios registrados.
-4. Los usuarios estudiantes deben ser redirigidos a sus respectivas páginas de inicio después de iniciar sesión.
-5. En caso de credenciales incorrectas, el sistema debe mostrar un mensaje de error apropiado y no permitir el acceso.
-6. Los usuarios deben poder cerrar la sesión de manera segura y regresar a la página de inicio de sesión.</t>
-  </si>
-  <si>
     <t>1. El sistema debe proporcionar un campo de entrada de usuario y contraseña en la página de inicio de sesión.
 2. Los usuarios deben poder ingresar su correo y contraseña en los campos correspondientes.
 3. El sistema debe verificar las credenciales proporcionadas por el usuario y autenticar con éxito a los usuarios registrados.
@@ -188,30 +173,61 @@
 6. Los usuarios deben poder cerrar la sesión de manera segura y regresar a la página de inicio de sesión.</t>
   </si>
   <si>
-    <t>El usuario Director de Trabajo de Grado debe poder iniciar sesión en la aplicación para poder acceder a sus funcionalidades.</t>
+    <t>CP09</t>
+  </si>
+  <si>
+    <t>CP011</t>
+  </si>
+  <si>
+    <t>El usuario Profesor debe poder crear propuestas de trabajo de grado, de modo que estas se publiquen.</t>
+  </si>
+  <si>
+    <t>Un profesor o usuario con los permisos de director de trabajo debe poder registrar el anteproyecto en el sistema</t>
+  </si>
+  <si>
+    <t>1. Los usuarios con rol Profesor deben poder acceder a la funcionalidad de crear Propuestas de trabajo de grado desde la interfaz de la aplicación.
+2.La interfaz de usuario debe ser intuitiva y amigable, permitiendo a los usuarios realizar las acciones de manera eficiente.</t>
+  </si>
+  <si>
+    <t>El coordinador o director del trabajo de grado debe poder ingresar los datos necesarios para registrar (enviar) el trabajo de grado.</t>
+  </si>
+  <si>
+    <t>1. Los usuarios con rol Profesor deben poder acceder a la funcionalidad de crear anteproyectos desde la interfaz de la aplicación.
+2.Todos los campos obligatorios se validan correctamente durante el registro.
+3.El sistema proporciona mensajes de error comprensibles.
+4.Después de completar todos los campos requeridos, el sistema permite el registro exitoso del anteproyecto.
+5.La interfaz de usuario debe ser intuitiva y amigable, permitiendo a los usuarios realizar las acciones de manera eficiente.</t>
+  </si>
+  <si>
+    <t>1. Los usuarios con rol Profesor deben poder acceder a la funcionalidad de crear trabajo de grado desde la interfaz de la aplicación.
+2.Todos los campos obligatorios se validan correctamente durante el registro.
+3.El sistema proporciona mensajes de error comprensibles.
+4.Después de completar todos los campos requeridos, el sistema permite el registro exitoso del Trabajo de grado.
+5.La interfaz de usuario debe ser intuitiva y amigable, permitiendo a los usuarios realizar las acciones de manera eficiente.</t>
+  </si>
+  <si>
+    <t>El usuario autorizado y con rol del concejo de facultad debe poder seleccionar el documento de la resolución de aprobación del anteproyecto especifico y subirlo al sistema.</t>
+  </si>
+  <si>
+    <t>CP013</t>
+  </si>
+  <si>
+    <t>El usuario autorizado y con rol del concejo de facultad debe poder iniciar sesión en la aplicación para poder acceder a sus funcionalidades.</t>
   </si>
   <si>
     <t>1. El sistema debe proporcionar un campo de entrada de usuario y contraseña en la página de inicio de sesión.
 2. Los usuarios deben poder ingresar su correo y contraseña en los campos correspondientes.
 3. El sistema debe verificar las credenciales proporcionadas por el usuario y autenticar con éxito a los usuarios registrados.
-4. Los usuarios Director de trabajo de grado deben ser redirigidos a sus respectivas páginas de inicio después de iniciar sesión.
+4. Los usuarios con rol de concejo de facultad deben ser redirigidos a sus respectivas páginas de inicio después de iniciar sesión.
 5. En caso de credenciales incorrectas, el sistema debe mostrar un mensaje de error apropiado y no permitir el acceso.
 6. Los usuarios deben poder cerrar la sesión de manera segura y regresar a la página de inicio de sesión.</t>
   </si>
   <si>
-    <t>CP09</t>
-  </si>
-  <si>
-    <t>CP011</t>
-  </si>
-  <si>
-    <t>El usuario Profesor debe poder crear propuestas de trabajo de grado, de modo que estas se publiquen.</t>
-  </si>
-  <si>
-    <t>El usuario director del trabajo de grado debe poder registrar los datos necesarios para registrar (enviar) el trabajo de grado.</t>
-  </si>
-  <si>
-    <t>Un profesor o usuario con los permisos de director de trabajo debe poder registrar el anteproyecto en el sistema</t>
+    <t>1. Los usuarios con rol de concejo de facultad deben poder acceder a la funcionalidad de subir la resolucion de aprobacion de el trabajo de grado que se seleccione desde la interfaz de la aplicación.
+2.La interfaz para seleccionar y subir el documento de resolución es clara y fácil de entender para el usuario del concejo de facultad.
+3.El sistema permite al usuario seleccionar el documento de la resolución de aprobación de un anteproyecto específico de manera clara y sencilla.
+4.Después de seleccionar el documento, el sistema permite subirlo exitosamente al sistema.
+5.La interfaz de usuario debe ser intuitiva y amigable, permitiendo a los usuarios realizar las acciones de manera eficiente.</t>
   </si>
 </sst>
 </file>
@@ -432,29 +448,29 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -773,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3AB2670-8968-4A3C-AF22-2617AA9D597B}">
   <dimension ref="B2:I18"/>
   <sheetViews>
-    <sheetView zoomScale="52" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A11" zoomScale="75" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -788,129 +804,127 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="2:9" ht="16.5">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" spans="2:9" ht="16.5">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="5" spans="2:9" ht="16.5">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
     </row>
     <row r="8" spans="2:9" ht="18.75" thickBot="1">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
     </row>
     <row r="9" spans="2:9" s="5" customFormat="1" ht="54" customHeight="1" thickTop="1">
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="13"/>
+      <c r="C9" s="14"/>
       <c r="D9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11" t="s">
+      <c r="G9" s="15"/>
+      <c r="H9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="11"/>
+      <c r="I9" s="15"/>
     </row>
     <row r="10" spans="2:9" ht="89.25">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="14"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
     </row>
     <row r="11" spans="2:9" ht="89.25">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="14"/>
+      <c r="C11" s="9"/>
       <c r="D11" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
     </row>
     <row r="12" spans="2:9" ht="16.5">
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="3"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
     </row>
     <row r="13" spans="2:9" ht="191.25">
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="14"/>
+      <c r="C13" s="9"/>
       <c r="D13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
     </row>
     <row r="15" spans="2:9" ht="15.75">
       <c r="B15" s="2" t="s">
@@ -939,12 +953,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H11:I11"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B9:C9"/>
@@ -953,12 +966,13 @@
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H11:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -969,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2633ACA9-8603-4095-B2DA-7E9864DEC261}">
   <dimension ref="B2:I18"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="65" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="57" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -984,121 +998,135 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="2:9" ht="16.5">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" spans="2:9" ht="16.5">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="5" spans="2:9" ht="16.5">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
     </row>
     <row r="8" spans="2:9" ht="18.75" thickBot="1">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
     </row>
     <row r="9" spans="2:9" s="5" customFormat="1" ht="54" customHeight="1" thickTop="1">
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="13"/>
+      <c r="C9" s="14"/>
       <c r="D9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11" t="s">
+      <c r="G9" s="15"/>
+      <c r="H9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="11"/>
+      <c r="I9" s="15"/>
     </row>
     <row r="10" spans="2:9" ht="89.25">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="14"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+    </row>
+    <row r="11" spans="2:9" ht="89.25">
+      <c r="B11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="10"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+    </row>
+    <row r="12" spans="2:9" ht="89.25">
+      <c r="B12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+    </row>
+    <row r="13" spans="2:9" ht="51">
+      <c r="B13" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="E13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-    </row>
-    <row r="11" spans="2:9" ht="42.75">
-      <c r="B11" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-    </row>
-    <row r="12" spans="2:9" ht="16.5">
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-    </row>
-    <row r="13" spans="2:9" ht="16.5">
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
     </row>
     <row r="14" spans="2:9">
       <c r="E14" s="8"/>
@@ -1130,6 +1158,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="H11:I11"/>
@@ -1144,23 +1178,17 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23D5C2DF-D057-40E2-BCBB-E8ADBBB80A86}">
-  <dimension ref="B2:I18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F14AD65-0BF0-4F9E-8729-C3B71F7205F6}">
+  <dimension ref="B2:I17"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A9" zoomScale="95" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1174,321 +1202,140 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="2:9" ht="16.5">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" spans="2:9" ht="16.5">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="5" spans="2:9" ht="16.5">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
     </row>
     <row r="8" spans="2:9" ht="18.75" thickBot="1">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
     </row>
     <row r="9" spans="2:9" s="5" customFormat="1" ht="54" customHeight="1" thickTop="1">
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="13"/>
+      <c r="C9" s="14"/>
       <c r="D9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11" t="s">
+      <c r="G9" s="15"/>
+      <c r="H9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="11"/>
-    </row>
-    <row r="10" spans="2:9" ht="89.25">
-      <c r="B10" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="14"/>
+      <c r="I9" s="15"/>
+    </row>
+    <row r="10" spans="2:9" ht="102">
+      <c r="B10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="9"/>
       <c r="D10" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-    </row>
-    <row r="11" spans="2:9" ht="16.5">
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="9" t="s">
+      <c r="G10" s="10"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+    </row>
+    <row r="11" spans="2:9" ht="128.25" customHeight="1">
+      <c r="B11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-    </row>
-    <row r="13" spans="2:9" ht="16.5">
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-    </row>
-    <row r="15" spans="2:9" ht="15.75">
-      <c r="B15" s="2" t="s">
+      <c r="G11" s="10"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+    </row>
+    <row r="12" spans="2:9" ht="16.5">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+    </row>
+    <row r="14" spans="2:9" ht="15.75">
+      <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="2:9">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="18" spans="2:6" ht="15.75">
-      <c r="B18" s="2" t="s">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="17" spans="2:6" ht="15.75">
+      <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B9:C9"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F14AD65-0BF0-4F9E-8729-C3B71F7205F6}">
-  <dimension ref="B2:I18"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="79" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="42.42578125" customWidth="1"/>
-    <col min="5" max="5" width="97.85546875" customWidth="1"/>
-    <col min="9" max="9" width="40.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:9" ht="16.5">
-      <c r="B2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-    </row>
-    <row r="3" spans="2:9" ht="16.5">
-      <c r="B3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4" spans="2:9" ht="16.5">
-      <c r="B4" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5" spans="2:9" ht="16.5">
-      <c r="B5" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="8" spans="2:9" ht="18.75" thickBot="1">
-      <c r="B8" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-    </row>
-    <row r="9" spans="2:9" s="5" customFormat="1" ht="54" customHeight="1" thickTop="1">
-      <c r="B9" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="11"/>
-    </row>
-    <row r="10" spans="2:9" ht="102">
-      <c r="B10" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-    </row>
-    <row r="11" spans="2:9" ht="61.5" customHeight="1">
-      <c r="B11" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-    </row>
-    <row r="12" spans="2:9" ht="68.25" customHeight="1">
-      <c r="B12" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-    </row>
-    <row r="13" spans="2:9" ht="16.5">
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-    </row>
-    <row r="15" spans="2:9" ht="15.75">
-      <c r="B15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="2:9">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="18" spans="2:6" ht="15.75">
-      <c r="B18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="20">
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="H11:I11"/>
@@ -1503,12 +1350,6 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modificacion de documento de Pruebas de aceptacion 30/11/23
</commit_message>
<xml_diff>
--- a/Tester/SRSPG_Pruebas_de_Aceptación.xlsx
+++ b/Tester/SRSPG_Pruebas_de_Aceptación.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanC\OneDrive\Escritorio\2023.2\proyecto 1\Proyecto-I\Tester\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanC\OneDrive\Escritorio\proyecto1\Proyecto-I\Tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8247088E-D73A-451A-BA14-D6263ED87F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9815562E-F50A-4138-92CE-61DBFAF46C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{9370D1F1-6C14-4FB8-9272-9D8C43E5B414}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{9370D1F1-6C14-4FB8-9272-9D8C43E5B414}"/>
   </bookViews>
   <sheets>
     <sheet name="PruebasAceptacion_Jefatura" sheetId="1" r:id="rId1"/>
@@ -112,20 +112,7 @@
     <t>CP06</t>
   </si>
   <si>
-    <t>El usuario Auxiliar de Jefatura y/o el jefe del departamento deben poder modificar el seguimiento creado automáticamente por el director del trabajo de grado al momento de crear el anteproyecto, se le debe permitir agregar o modificar fechas, observaciones y cambiar el estado del anteproyecto.</t>
-  </si>
-  <si>
     <t>Pendiente</t>
-  </si>
-  <si>
-    <t>1. Los usuarios Auxiliar de Jefatura y jefe del departamento deben poder acceder a la funcionalidad de modificación del seguimiento desde la interfaz de la aplicación.
-2. La funcionalidad de modificación del seguimiento debe proporcionar la capacidad de seleccionar un anteproyecto específico al que desean realizar modificaciones.
-3. Deben poder agregar nuevas fechas de seguimiento al anteproyecto, especificando la fecha y una descripción de la actividad asociada.
-4. Los usuarios deben poder modificar las fechas de seguimiento existentes, incluyendo la capacidad de cambiar la fecha y la descripción de la actividad.
-5. Deben poder agregar observaciones relacionadas con el anteproyecto y las actividades de seguimiento.
-6. Los usuarios deben tener la capacidad de cambiar el estado del anteproyecto, como "En Progreso," "Completado" o "En Revisión.".
-7. La modificación del seguimiento no debe afectar negativamente la integridad de los datos ni causar errores en la aplicación.
-8.La interfaz de usuario debe ser intuitiva y amigable, permitiendo a los usuarios realizar las modificaciones de manera eficiente.</t>
   </si>
   <si>
     <t>El usuario Auxiliar de Jefatura debe poder iniciar sesión en la aplicación para poder acceder a sus funcionalidades.</t>
@@ -228,6 +215,16 @@
 3.El sistema permite al usuario seleccionar el documento de la resolución de aprobación de un anteproyecto específico de manera clara y sencilla.
 4.Después de seleccionar el documento, el sistema permite subirlo exitosamente al sistema.
 5.La interfaz de usuario debe ser intuitiva y amigable, permitiendo a los usuarios realizar las acciones de manera eficiente.</t>
+  </si>
+  <si>
+    <t>El usuario Auxiliar de Jefatura y/o el jefe del departamento deben poder modificar el seguimiento creado automáticamente por el director del trabajo de grado al momento de crear el anteproyecto, se le debe permitir modificar el estado del seguimieto.</t>
+  </si>
+  <si>
+    <t>1. Los usuarios Auxiliar de Jefatura y jefe del departamento deben poder acceder a la funcionalidad de modificación del seguimiento desde la interfaz de la aplicación.
+2. La funcionalidad de modificación del seguimiento debe proporcionar la capacidad de seleccionar un anteproyecto específico al que desean realizar modificaciones.
+3. Los usuarios deben poder asignar los dos evaluadores al anteproyecto especifico y cambiar su estado a "en revision" y viceversa.
+4. La modificación del seguimiento no debe afectar negativamente la integridad de los datos ni causar errores en la aplicación.
+5. La interfaz de usuario debe ser intuitiva y amigable, permitiendo a los usuarios realizar las modificaciones de manera eficiente.</t>
   </si>
 </sst>
 </file>
@@ -789,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3AB2670-8968-4A3C-AF22-2617AA9D597B}">
   <dimension ref="B2:I18"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="75" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView zoomScale="104" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -864,17 +861,17 @@
     </row>
     <row r="10" spans="2:9" ht="89.25">
       <c r="B10" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="16"/>
@@ -882,17 +879,17 @@
     </row>
     <row r="11" spans="2:9" ht="89.25">
       <c r="B11" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="16"/>
@@ -908,19 +905,19 @@
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
     </row>
-    <row r="13" spans="2:9" ht="191.25">
+    <row r="13" spans="2:9" ht="127.5">
       <c r="B13" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>15</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="16"/>
@@ -983,7 +980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2633ACA9-8603-4095-B2DA-7E9864DEC261}">
   <dimension ref="B2:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="57" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="68" workbookViewId="0">
       <selection activeCell="B13" sqref="B13:C13"/>
     </sheetView>
   </sheetViews>
@@ -1062,13 +1059,13 @@
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="16"/>
@@ -1076,17 +1073,17 @@
     </row>
     <row r="11" spans="2:9" ht="89.25">
       <c r="B11" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="16"/>
@@ -1094,17 +1091,17 @@
     </row>
     <row r="12" spans="2:9" ht="89.25">
       <c r="B12" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>34</v>
-      </c>
       <c r="F12" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="16"/>
@@ -1112,17 +1109,17 @@
     </row>
     <row r="13" spans="2:9" ht="51">
       <c r="B13" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>31</v>
-      </c>
       <c r="F13" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="16"/>
@@ -1187,7 +1184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F14AD65-0BF0-4F9E-8729-C3B71F7205F6}">
   <dimension ref="B2:I17"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="95" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="95" workbookViewId="0">
       <selection activeCell="F12" sqref="F12:G12"/>
     </sheetView>
   </sheetViews>
@@ -1266,13 +1263,13 @@
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="16"/>
@@ -1280,17 +1277,17 @@
     </row>
     <row r="11" spans="2:9" ht="128.25" customHeight="1">
       <c r="B11" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="16"/>

</xml_diff>

<commit_message>
Modificacion de documento de Pruebas 04/12/23
</commit_message>
<xml_diff>
--- a/Tester/SRSPG_Pruebas_de_Aceptación.xlsx
+++ b/Tester/SRSPG_Pruebas_de_Aceptación.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanC\OneDrive\Escritorio\proyecto1\Proyecto-I\Tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9815562E-F50A-4138-92CE-61DBFAF46C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D63B53-6DDE-4C3E-AF37-70CE031A5622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{9370D1F1-6C14-4FB8-9272-9D8C43E5B414}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{9370D1F1-6C14-4FB8-9272-9D8C43E5B414}"/>
   </bookViews>
   <sheets>
     <sheet name="PruebasAceptacion_Jefatura" sheetId="1" r:id="rId1"/>
@@ -38,12 +38,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="42">
   <si>
     <t>Número del Caso de Prueba</t>
-  </si>
-  <si>
-    <t>Fecha de Finalaizacion de las pruebas:</t>
   </si>
   <si>
     <r>
@@ -226,6 +223,25 @@
 4. La modificación del seguimiento no debe afectar negativamente la integridad de los datos ni causar errores en la aplicación.
 5. La interfaz de usuario debe ser intuitiva y amigable, permitiendo a los usuarios realizar las modificaciones de manera eficiente.</t>
   </si>
+  <si>
+    <t>Auxiliar administrativo de jefatura:</t>
+  </si>
+  <si>
+    <t>Aprobada</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fecha de Finalaizacion de las pruebas: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="NewsGotT"/>
+      </rPr>
+      <t>1/12/23</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -234,7 +250,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,6 +324,14 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -421,7 +445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -445,6 +469,18 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -457,17 +493,8 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -485,6 +512,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3767442</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>63539</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF881C60-82B2-4073-B316-50A92E50780D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="247284" y="7812332"/>
+          <a:ext cx="7788091" cy="3525510"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -784,10 +860,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3AB2670-8968-4A3C-AF22-2617AA9D597B}">
-  <dimension ref="B2:I18"/>
+  <dimension ref="B2:I20"/>
   <sheetViews>
     <sheetView zoomScale="104" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B4" sqref="B4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -801,131 +877,131 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="2:9" ht="16.5">
+      <c r="B3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-    </row>
-    <row r="3" spans="2:9" ht="16.5">
-      <c r="B3" s="13" t="s">
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="2:9" ht="16.5">
+      <c r="B4" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="2:9" ht="16.5">
+      <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-    </row>
-    <row r="4" spans="2:9" ht="16.5">
-      <c r="B4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-    </row>
-    <row r="5" spans="2:9" ht="16.5">
-      <c r="B5" s="13" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+    </row>
+    <row r="8" spans="2:9" ht="18.75" thickBot="1">
+      <c r="B8" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-    </row>
-    <row r="8" spans="2:9" ht="18.75" thickBot="1">
-      <c r="B8" s="11" t="s">
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="2:9" s="5" customFormat="1" ht="54" customHeight="1" thickTop="1">
+      <c r="B9" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="2:9" s="5" customFormat="1" ht="54" customHeight="1" thickTop="1">
-      <c r="B9" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="G9" s="10"/>
+      <c r="H9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="15"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" spans="2:9" ht="89.25">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="2:9" ht="89.25">
+      <c r="B11" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-    </row>
-    <row r="11" spans="2:9" ht="89.25">
-      <c r="B11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
+      <c r="F11" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
     </row>
     <row r="12" spans="2:9" ht="16.5">
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="3"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
     </row>
     <row r="13" spans="2:9" ht="127.5">
-      <c r="B13" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="9"/>
+      <c r="B13" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="13"/>
       <c r="D13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
+      <c r="F13" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
     </row>
     <row r="15" spans="2:9" ht="15.75">
       <c r="B15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -941,20 +1017,30 @@
     </row>
     <row r="18" spans="2:6" ht="15.75">
       <c r="B18" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
+    <row r="20" spans="2:6" ht="15" customHeight="1">
+      <c r="B20" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+    </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H11:I11"/>
+  <mergeCells count="21">
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="F12:G12"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B9:C9"/>
@@ -963,16 +1049,15 @@
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H11:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -981,7 +1066,7 @@
   <dimension ref="B2:I18"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="68" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:C13"/>
+      <selection activeCell="B4" sqref="B4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -995,142 +1080,142 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="2:9" ht="16.5">
+      <c r="B3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-    </row>
-    <row r="3" spans="2:9" ht="16.5">
-      <c r="B3" s="13" t="s">
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="2:9" ht="16.5">
+      <c r="B4" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="2:9" ht="16.5">
+      <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-    </row>
-    <row r="4" spans="2:9" ht="16.5">
-      <c r="B4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-    </row>
-    <row r="5" spans="2:9" ht="16.5">
-      <c r="B5" s="13" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+    </row>
+    <row r="8" spans="2:9" ht="18.75" thickBot="1">
+      <c r="B8" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-    </row>
-    <row r="8" spans="2:9" ht="18.75" thickBot="1">
-      <c r="B8" s="11" t="s">
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="2:9" s="5" customFormat="1" ht="54" customHeight="1" thickTop="1">
+      <c r="B9" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="2:9" s="5" customFormat="1" ht="54" customHeight="1" thickTop="1">
-      <c r="B9" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="G9" s="10"/>
+      <c r="H9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="15"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" spans="2:9" ht="89.25">
-      <c r="B10" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="9"/>
+      <c r="B10" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="13"/>
       <c r="D10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="2:9" ht="89.25">
+      <c r="B11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-    </row>
-    <row r="11" spans="2:9" ht="89.25">
-      <c r="B11" s="9" t="s">
+      <c r="C11" s="13"/>
+      <c r="D11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="2:9" ht="89.25">
+      <c r="B12" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="3" t="s">
+      <c r="C12" s="13"/>
+      <c r="D12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="2:9" ht="51">
+      <c r="B13" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-    </row>
-    <row r="12" spans="2:9" ht="89.25">
-      <c r="B12" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-    </row>
-    <row r="13" spans="2:9" ht="51">
-      <c r="B13" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
+      <c r="F13" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
     </row>
     <row r="14" spans="2:9">
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="2:9" ht="15.75">
       <c r="B15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1146,7 +1231,7 @@
     </row>
     <row r="18" spans="2:6" ht="15.75">
       <c r="B18" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1155,12 +1240,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="H11:I11"/>
@@ -1175,6 +1254,12 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1184,8 +1269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F14AD65-0BF0-4F9E-8729-C3B71F7205F6}">
   <dimension ref="B2:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="95" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12:G12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="58" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1199,113 +1284,113 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16.5">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="2:9" ht="16.5">
+      <c r="B3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-    </row>
-    <row r="3" spans="2:9" ht="16.5">
-      <c r="B3" s="13" t="s">
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="2:9" ht="16.5">
+      <c r="B4" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="2:9" ht="16.5">
+      <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-    </row>
-    <row r="4" spans="2:9" ht="16.5">
-      <c r="B4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-    </row>
-    <row r="5" spans="2:9" ht="16.5">
-      <c r="B5" s="13" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+    </row>
+    <row r="8" spans="2:9" ht="18.75" thickBot="1">
+      <c r="B8" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-    </row>
-    <row r="8" spans="2:9" ht="18.75" thickBot="1">
-      <c r="B8" s="11" t="s">
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="2:9" s="5" customFormat="1" ht="54" customHeight="1" thickTop="1">
+      <c r="B9" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="2:9" s="5" customFormat="1" ht="54" customHeight="1" thickTop="1">
-      <c r="B9" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="G9" s="10"/>
+      <c r="H9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="15"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" spans="2:9" ht="102">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="G10" s="14"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="2:9" ht="128.25" customHeight="1">
+      <c r="B11" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-    </row>
-    <row r="11" spans="2:9" ht="128.25" customHeight="1">
-      <c r="B11" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
+      <c r="F11" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
     </row>
     <row r="12" spans="2:9" ht="16.5">
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="3"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
     </row>
     <row r="14" spans="2:9" ht="15.75">
       <c r="B14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1321,7 +1406,7 @@
     </row>
     <row r="17" spans="2:6" ht="15.75">
       <c r="B17" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1330,23 +1415,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B8:D8"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>